<commit_message>
drug mapping between DrugBankID and originally provided compound names
</commit_message>
<xml_diff>
--- a/data/Table of compounds_whole_2025-06-13.xlsx
+++ b/data/Table of compounds_whole_2025-06-13.xlsx
@@ -3206,6 +3206,147 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="61" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3227,9 +3368,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3257,15 +3395,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3319,168 +3448,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="61" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3519,6 +3492,33 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3543,16 +3543,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5235404-1F3C-4F5D-8BD1-38EC52CC3506}" name="Table3" displayName="Table3" ref="A1:G26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5235404-1F3C-4F5D-8BD1-38EC52CC3506}" name="Table3" displayName="Table3" ref="A1:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G26" xr:uid="{F5235404-1F3C-4F5D-8BD1-38EC52CC3506}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{17692C5A-7271-4FC3-AC90-87DB148CFA80}" name="Filename" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5E4C95EF-1CA2-4E4F-A028-A35DB7D17E83}" name="Batch_ID" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8FE15845-ED69-42B6-B60D-4594D594EB53}" name="Date" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{1189E5F9-77C9-4D24-9A02-A42C87B63283}" name="Run date" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{F5663A89-2907-4B4B-96C2-6D7E9C6218E7}" name="Num Barcode IDs" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{FBF26A8E-CB6E-4084-AEB9-CAB98566E14E}" name="Num Replicates" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{E3EF40AB-A7B2-425E-9295-3CEB9A3DABF6}" name="General Comments Per Batch" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{17692C5A-7271-4FC3-AC90-87DB148CFA80}" name="Filename" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{5E4C95EF-1CA2-4E4F-A028-A35DB7D17E83}" name="Batch_ID" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{8FE15845-ED69-42B6-B60D-4594D594EB53}" name="Date" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1189E5F9-77C9-4D24-9A02-A42C87B63283}" name="Run date" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F5663A89-2907-4B4B-96C2-6D7E9C6218E7}" name="Num Barcode IDs" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FBF26A8E-CB6E-4084-AEB9-CAB98566E14E}" name="Num Replicates" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E3EF40AB-A7B2-425E-9295-3CEB9A3DABF6}" name="General Comments Per Batch" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3580,8 +3580,8 @@
     <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Compound" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0569DB07-56D4-46A1-8998-DAE8B18F7DD3}" name="Samples_ID" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Compound" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{0569DB07-56D4-46A1-8998-DAE8B18F7DD3}" name="Samples_ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3903,13 +3903,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="405" t="s">
+      <c r="A2" s="348" t="s">
         <v>372</v>
       </c>
-      <c r="B2" s="405" t="s">
+      <c r="B2" s="348" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="405" t="s">
+      <c r="C2" s="348" t="s">
         <v>372</v>
       </c>
       <c r="D2" s="4">
@@ -3933,9 +3933,9 @@
       <c r="J2" s="320"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="406"/>
-      <c r="B3" s="406"/>
-      <c r="C3" s="406"/>
+      <c r="A3" s="349"/>
+      <c r="B3" s="349"/>
+      <c r="C3" s="349"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
@@ -3957,9 +3957,9 @@
       <c r="J3" s="321"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="406"/>
-      <c r="B4" s="406"/>
-      <c r="C4" s="406"/>
+      <c r="A4" s="349"/>
+      <c r="B4" s="349"/>
+      <c r="C4" s="349"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -3981,9 +3981,9 @@
       <c r="J4" s="321"/>
     </row>
     <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="406"/>
-      <c r="B5" s="406"/>
-      <c r="C5" s="406"/>
+      <c r="A5" s="349"/>
+      <c r="B5" s="349"/>
+      <c r="C5" s="349"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4007,9 +4007,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="406"/>
-      <c r="B6" s="406"/>
-      <c r="C6" s="406"/>
+      <c r="A6" s="349"/>
+      <c r="B6" s="349"/>
+      <c r="C6" s="349"/>
       <c r="D6" s="5" t="s">
         <v>373</v>
       </c>
@@ -4031,9 +4031,9 @@
       <c r="J6" s="321"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="406"/>
-      <c r="B7" s="406"/>
-      <c r="C7" s="406"/>
+      <c r="A7" s="349"/>
+      <c r="B7" s="349"/>
+      <c r="C7" s="349"/>
       <c r="D7" s="5" t="s">
         <v>373</v>
       </c>
@@ -4055,9 +4055,9 @@
       <c r="J7" s="321"/>
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="406"/>
-      <c r="B8" s="406"/>
-      <c r="C8" s="406"/>
+      <c r="A8" s="349"/>
+      <c r="B8" s="349"/>
+      <c r="C8" s="349"/>
       <c r="D8" s="322" t="s">
         <v>373</v>
       </c>
@@ -4081,9 +4081,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="406"/>
-      <c r="B9" s="406"/>
-      <c r="C9" s="406"/>
+      <c r="A9" s="349"/>
+      <c r="B9" s="349"/>
+      <c r="C9" s="349"/>
       <c r="D9" t="s">
         <v>373</v>
       </c>
@@ -4107,9 +4107,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="406"/>
-      <c r="B10" s="406"/>
-      <c r="C10" s="406"/>
+      <c r="A10" s="349"/>
+      <c r="B10" s="349"/>
+      <c r="C10" s="349"/>
       <c r="D10" s="323" t="s">
         <v>373</v>
       </c>
@@ -4131,9 +4131,9 @@
       <c r="J10" s="325"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="407"/>
-      <c r="B11" s="407"/>
-      <c r="C11" s="407"/>
+      <c r="A11" s="350"/>
+      <c r="B11" s="350"/>
+      <c r="C11" s="350"/>
       <c r="D11" s="326" t="s">
         <v>373</v>
       </c>
@@ -4155,13 +4155,13 @@
       <c r="J11" s="327"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="408" t="s">
+      <c r="A12" s="351" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="408" t="s">
+      <c r="B12" s="351" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="405" t="s">
+      <c r="C12" s="348" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -4185,9 +4185,9 @@
       <c r="J12" s="247"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="409"/>
-      <c r="B13" s="409"/>
-      <c r="C13" s="428"/>
+      <c r="A13" s="352"/>
+      <c r="B13" s="352"/>
+      <c r="C13" s="373"/>
       <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
@@ -4208,9 +4208,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="409"/>
-      <c r="B14" s="409"/>
-      <c r="C14" s="428"/>
+      <c r="A14" s="352"/>
+      <c r="B14" s="352"/>
+      <c r="C14" s="373"/>
       <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
@@ -4232,9 +4232,9 @@
       <c r="J14" s="248"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="409"/>
-      <c r="B15" s="409"/>
-      <c r="C15" s="428"/>
+      <c r="A15" s="352"/>
+      <c r="B15" s="352"/>
+      <c r="C15" s="373"/>
       <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
@@ -4256,9 +4256,9 @@
       <c r="J15" s="248"/>
     </row>
     <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="409"/>
-      <c r="B16" s="409"/>
-      <c r="C16" s="428"/>
+      <c r="A16" s="352"/>
+      <c r="B16" s="352"/>
+      <c r="C16" s="373"/>
       <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
@@ -4280,9 +4280,9 @@
       <c r="J16" s="248"/>
     </row>
     <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="409"/>
-      <c r="B17" s="409"/>
-      <c r="C17" s="428"/>
+      <c r="A17" s="352"/>
+      <c r="B17" s="352"/>
+      <c r="C17" s="373"/>
       <c r="D17" s="5" t="s">
         <v>17</v>
       </c>
@@ -4306,9 +4306,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="409"/>
-      <c r="B18" s="409"/>
-      <c r="C18" s="428"/>
+      <c r="A18" s="352"/>
+      <c r="B18" s="352"/>
+      <c r="C18" s="373"/>
       <c r="D18" s="8" t="s">
         <v>17</v>
       </c>
@@ -4330,9 +4330,9 @@
       <c r="J18" s="250"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="409"/>
-      <c r="B19" s="409"/>
-      <c r="C19" s="428"/>
+      <c r="A19" s="352"/>
+      <c r="B19" s="352"/>
+      <c r="C19" s="373"/>
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -4354,9 +4354,9 @@
       <c r="J19" s="251"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="409"/>
-      <c r="B20" s="409"/>
-      <c r="C20" s="428"/>
+      <c r="A20" s="352"/>
+      <c r="B20" s="352"/>
+      <c r="C20" s="373"/>
       <c r="D20" s="19" t="s">
         <v>17</v>
       </c>
@@ -4378,9 +4378,9 @@
       <c r="J20" s="252"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="409"/>
-      <c r="B21" s="409"/>
-      <c r="C21" s="428"/>
+      <c r="A21" s="352"/>
+      <c r="B21" s="352"/>
+      <c r="C21" s="373"/>
       <c r="D21" s="113" t="s">
         <v>17</v>
       </c>
@@ -4402,9 +4402,9 @@
       <c r="J21" s="253"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="409"/>
-      <c r="B22" s="409"/>
-      <c r="C22" s="428"/>
+      <c r="A22" s="352"/>
+      <c r="B22" s="352"/>
+      <c r="C22" s="373"/>
       <c r="D22" s="98" t="s">
         <v>18</v>
       </c>
@@ -4428,9 +4428,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="409"/>
-      <c r="B23" s="409"/>
-      <c r="C23" s="428"/>
+      <c r="A23" s="352"/>
+      <c r="B23" s="352"/>
+      <c r="C23" s="373"/>
       <c r="D23" s="16" t="s">
         <v>17</v>
       </c>
@@ -4452,8 +4452,8 @@
       <c r="J23" s="252"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="409"/>
-      <c r="B24" s="409"/>
+      <c r="A24" s="352"/>
+      <c r="B24" s="352"/>
       <c r="C24" s="331" t="s">
         <v>406</v>
       </c>
@@ -4480,8 +4480,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="409"/>
-      <c r="B25" s="409"/>
+      <c r="A25" s="352"/>
+      <c r="B25" s="352"/>
       <c r="C25" s="331" t="s">
         <v>404</v>
       </c>
@@ -4508,8 +4508,8 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="409"/>
-      <c r="B26" s="409"/>
+      <c r="A26" s="352"/>
+      <c r="B26" s="352"/>
       <c r="C26" s="331" t="s">
         <v>405</v>
       </c>
@@ -4536,8 +4536,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="409"/>
-      <c r="B27" s="409"/>
+      <c r="A27" s="352"/>
+      <c r="B27" s="352"/>
       <c r="C27" s="331" t="s">
         <v>16</v>
       </c>
@@ -4564,13 +4564,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="417" t="s">
+      <c r="A28" s="362" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="410" t="s">
+      <c r="B28" s="353" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="420" t="s">
+      <c r="C28" s="365" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="99" t="s">
@@ -4596,9 +4596,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="418"/>
-      <c r="B29" s="411"/>
-      <c r="C29" s="421"/>
+      <c r="A29" s="363"/>
+      <c r="B29" s="354"/>
+      <c r="C29" s="366"/>
       <c r="D29" s="100" t="s">
         <v>17</v>
       </c>
@@ -4620,9 +4620,9 @@
       <c r="J29" s="257"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="418"/>
-      <c r="B30" s="411"/>
-      <c r="C30" s="421"/>
+      <c r="A30" s="363"/>
+      <c r="B30" s="354"/>
+      <c r="C30" s="366"/>
       <c r="D30" s="102" t="s">
         <v>17</v>
       </c>
@@ -4644,9 +4644,9 @@
       <c r="J30" s="249"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="418"/>
-      <c r="B31" s="411"/>
-      <c r="C31" s="421"/>
+      <c r="A31" s="363"/>
+      <c r="B31" s="354"/>
+      <c r="C31" s="366"/>
       <c r="D31" s="102" t="s">
         <v>17</v>
       </c>
@@ -4668,9 +4668,9 @@
       <c r="J31" s="249"/>
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="418"/>
-      <c r="B32" s="411"/>
-      <c r="C32" s="421"/>
+      <c r="A32" s="363"/>
+      <c r="B32" s="354"/>
+      <c r="C32" s="366"/>
       <c r="D32" s="102" t="s">
         <v>17</v>
       </c>
@@ -4694,9 +4694,9 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="418"/>
-      <c r="B33" s="411"/>
-      <c r="C33" s="421"/>
+      <c r="A33" s="363"/>
+      <c r="B33" s="354"/>
+      <c r="C33" s="366"/>
       <c r="D33" s="102" t="s">
         <v>17</v>
       </c>
@@ -4720,9 +4720,9 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="418"/>
-      <c r="B34" s="411"/>
-      <c r="C34" s="421"/>
+      <c r="A34" s="363"/>
+      <c r="B34" s="354"/>
+      <c r="C34" s="366"/>
       <c r="D34" s="102" t="s">
         <v>17</v>
       </c>
@@ -4746,9 +4746,9 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="418"/>
-      <c r="B35" s="411"/>
-      <c r="C35" s="421"/>
+      <c r="A35" s="363"/>
+      <c r="B35" s="354"/>
+      <c r="C35" s="366"/>
       <c r="D35" s="128" t="s">
         <v>17</v>
       </c>
@@ -4772,9 +4772,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="418"/>
-      <c r="B36" s="411"/>
-      <c r="C36" s="421"/>
+      <c r="A36" s="363"/>
+      <c r="B36" s="354"/>
+      <c r="C36" s="366"/>
       <c r="D36" s="128" t="s">
         <v>17</v>
       </c>
@@ -4798,9 +4798,9 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="418"/>
-      <c r="B37" s="411"/>
-      <c r="C37" s="421"/>
+      <c r="A37" s="363"/>
+      <c r="B37" s="354"/>
+      <c r="C37" s="366"/>
       <c r="D37" s="128" t="s">
         <v>17</v>
       </c>
@@ -4824,9 +4824,9 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="418"/>
-      <c r="B38" s="411"/>
-      <c r="C38" s="421"/>
+      <c r="A38" s="363"/>
+      <c r="B38" s="354"/>
+      <c r="C38" s="366"/>
       <c r="D38" s="128" t="s">
         <v>17</v>
       </c>
@@ -4850,9 +4850,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="418"/>
-      <c r="B39" s="411"/>
-      <c r="C39" s="421"/>
+      <c r="A39" s="363"/>
+      <c r="B39" s="354"/>
+      <c r="C39" s="366"/>
       <c r="D39" s="128" t="s">
         <v>17</v>
       </c>
@@ -4876,9 +4876,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="418"/>
-      <c r="B40" s="411"/>
-      <c r="C40" s="421"/>
+      <c r="A40" s="363"/>
+      <c r="B40" s="354"/>
+      <c r="C40" s="366"/>
       <c r="D40" s="128" t="s">
         <v>17</v>
       </c>
@@ -4902,9 +4902,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="418"/>
-      <c r="B41" s="411"/>
-      <c r="C41" s="422"/>
+      <c r="A41" s="363"/>
+      <c r="B41" s="354"/>
+      <c r="C41" s="367"/>
       <c r="D41" s="128" t="s">
         <v>17</v>
       </c>
@@ -4928,8 +4928,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="418"/>
-      <c r="B42" s="411"/>
+      <c r="A42" s="363"/>
+      <c r="B42" s="354"/>
       <c r="C42" s="110" t="s">
         <v>32</v>
       </c>
@@ -4956,8 +4956,8 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="418"/>
-      <c r="B43" s="411"/>
+      <c r="A43" s="363"/>
+      <c r="B43" s="354"/>
       <c r="C43" s="136" t="s">
         <v>197</v>
       </c>
@@ -4982,8 +4982,8 @@
       <c r="J43" s="259"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="418"/>
-      <c r="B44" s="411"/>
+      <c r="A44" s="363"/>
+      <c r="B44" s="354"/>
       <c r="C44" s="136" t="s">
         <v>198</v>
       </c>
@@ -5008,8 +5008,8 @@
       <c r="J44" s="259"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="418"/>
-      <c r="B45" s="411"/>
+      <c r="A45" s="363"/>
+      <c r="B45" s="354"/>
       <c r="C45" s="127" t="s">
         <v>199</v>
       </c>
@@ -5034,8 +5034,8 @@
       <c r="J45" s="260"/>
     </row>
     <row r="46" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="418"/>
-      <c r="B46" s="412"/>
+      <c r="A46" s="363"/>
+      <c r="B46" s="355"/>
       <c r="C46" s="174" t="s">
         <v>321</v>
       </c>
@@ -5062,11 +5062,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="418"/>
-      <c r="B47" s="425" t="s">
+      <c r="A47" s="363"/>
+      <c r="B47" s="370" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="426" t="s">
+      <c r="C47" s="371" t="s">
         <v>29</v>
       </c>
       <c r="D47" s="100" t="s">
@@ -5090,9 +5090,9 @@
       <c r="J47" s="257"/>
     </row>
     <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="418"/>
-      <c r="B48" s="423"/>
-      <c r="C48" s="426"/>
+      <c r="A48" s="363"/>
+      <c r="B48" s="368"/>
+      <c r="C48" s="371"/>
       <c r="D48" s="105" t="s">
         <v>17</v>
       </c>
@@ -5114,9 +5114,9 @@
       <c r="J48" s="261"/>
     </row>
     <row r="49" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="418"/>
-      <c r="B49" s="423"/>
-      <c r="C49" s="427"/>
+      <c r="A49" s="363"/>
+      <c r="B49" s="368"/>
+      <c r="C49" s="372"/>
       <c r="D49" s="173" t="s">
         <v>17</v>
       </c>
@@ -5140,8 +5140,8 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="418"/>
-      <c r="B50" s="423" t="s">
+      <c r="A50" s="363"/>
+      <c r="B50" s="368" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="130" t="s">
@@ -5168,8 +5168,8 @@
       <c r="J50" s="314"/>
     </row>
     <row r="51" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="419"/>
-      <c r="B51" s="424"/>
+      <c r="A51" s="364"/>
+      <c r="B51" s="369"/>
       <c r="C51" s="130" t="s">
         <v>132</v>
       </c>
@@ -5226,11 +5226,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="392" t="s">
+      <c r="A53" s="387" t="s">
         <v>35</v>
       </c>
       <c r="B53" s="178"/>
-      <c r="C53" s="389" t="s">
+      <c r="C53" s="360" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="57" t="s">
@@ -5254,9 +5254,9 @@
       <c r="J53" s="263"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="393"/>
+      <c r="A54" s="388"/>
       <c r="B54" s="178"/>
-      <c r="C54" s="390"/>
+      <c r="C54" s="361"/>
       <c r="D54" s="60" t="s">
         <v>17</v>
       </c>
@@ -5278,9 +5278,9 @@
       <c r="J54" s="264"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="393"/>
+      <c r="A55" s="388"/>
       <c r="B55" s="178"/>
-      <c r="C55" s="389" t="s">
+      <c r="C55" s="360" t="s">
         <v>36</v>
       </c>
       <c r="D55" s="57" t="s">
@@ -5304,9 +5304,9 @@
       <c r="J55" s="263"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="393"/>
+      <c r="A56" s="388"/>
       <c r="B56" s="178"/>
-      <c r="C56" s="390"/>
+      <c r="C56" s="361"/>
       <c r="D56" s="60" t="s">
         <v>17</v>
       </c>
@@ -5328,7 +5328,7 @@
       <c r="J56" s="264"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="393"/>
+      <c r="A57" s="388"/>
       <c r="B57" s="179"/>
       <c r="C57" s="143" t="s">
         <v>38</v>
@@ -5354,7 +5354,7 @@
       <c r="J57" s="265"/>
     </row>
     <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="394"/>
+      <c r="A58" s="389"/>
       <c r="B58" s="180"/>
       <c r="C58" s="64" t="s">
         <v>201</v>
@@ -5380,11 +5380,11 @@
       <c r="J58" s="266"/>
     </row>
     <row r="59" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="366" t="s">
+      <c r="A59" s="378" t="s">
         <v>43</v>
       </c>
       <c r="B59" s="181"/>
-      <c r="C59" s="391" t="s">
+      <c r="C59" s="386" t="s">
         <v>41</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5408,9 +5408,9 @@
       <c r="J59" s="267"/>
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="366"/>
+      <c r="A60" s="378"/>
       <c r="B60" s="181"/>
-      <c r="C60" s="391"/>
+      <c r="C60" s="386"/>
       <c r="D60" s="5" t="s">
         <v>17</v>
       </c>
@@ -5432,9 +5432,9 @@
       <c r="J60" s="248"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="366"/>
+      <c r="A61" s="378"/>
       <c r="B61" s="181"/>
-      <c r="C61" s="391"/>
+      <c r="C61" s="386"/>
       <c r="D61" s="8" t="s">
         <v>17</v>
       </c>
@@ -5456,7 +5456,7 @@
       <c r="J61" s="268"/>
     </row>
     <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="367"/>
+      <c r="A62" s="377"/>
       <c r="B62" s="182"/>
       <c r="C62" s="30" t="s">
         <v>45</v>
@@ -5482,7 +5482,7 @@
       <c r="J62" s="269"/>
     </row>
     <row r="63" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="358" t="s">
+      <c r="A63" s="404" t="s">
         <v>50</v>
       </c>
       <c r="B63" s="183" t="s">
@@ -5514,7 +5514,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="359"/>
+      <c r="A64" s="405"/>
       <c r="B64" s="184" t="s">
         <v>50</v>
       </c>
@@ -5574,13 +5574,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="368" t="s">
+      <c r="A66" s="411" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="373" t="s">
+      <c r="B66" s="416" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="378" t="s">
+      <c r="C66" s="421" t="s">
         <v>54</v>
       </c>
       <c r="D66" s="51" t="s">
@@ -5604,9 +5604,9 @@
       <c r="J66" s="273"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="369"/>
-      <c r="B67" s="374"/>
-      <c r="C67" s="379"/>
+      <c r="A67" s="412"/>
+      <c r="B67" s="417"/>
+      <c r="C67" s="422"/>
       <c r="D67" s="40" t="s">
         <v>17</v>
       </c>
@@ -5628,9 +5628,9 @@
       <c r="J67" s="274"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="369"/>
-      <c r="B68" s="374"/>
-      <c r="C68" s="379"/>
+      <c r="A68" s="412"/>
+      <c r="B68" s="417"/>
+      <c r="C68" s="422"/>
       <c r="D68" s="53" t="s">
         <v>17</v>
       </c>
@@ -5652,9 +5652,9 @@
       <c r="J68" s="275"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="369"/>
-      <c r="B69" s="375"/>
-      <c r="C69" s="379"/>
+      <c r="A69" s="412"/>
+      <c r="B69" s="418"/>
+      <c r="C69" s="422"/>
       <c r="D69" s="10" t="s">
         <v>17</v>
       </c>
@@ -5678,9 +5678,9 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="369"/>
-      <c r="B70" s="375"/>
-      <c r="C70" s="379"/>
+      <c r="A70" s="412"/>
+      <c r="B70" s="418"/>
+      <c r="C70" s="422"/>
       <c r="D70" s="10" t="s">
         <v>17</v>
       </c>
@@ -5704,9 +5704,9 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="369"/>
-      <c r="B71" s="375"/>
-      <c r="C71" s="379"/>
+      <c r="A71" s="412"/>
+      <c r="B71" s="418"/>
+      <c r="C71" s="422"/>
       <c r="D71" s="10" t="s">
         <v>17</v>
       </c>
@@ -5730,9 +5730,9 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="369"/>
-      <c r="B72" s="375"/>
-      <c r="C72" s="379"/>
+      <c r="A72" s="412"/>
+      <c r="B72" s="418"/>
+      <c r="C72" s="422"/>
       <c r="D72" s="10" t="s">
         <v>17</v>
       </c>
@@ -5756,9 +5756,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="369"/>
-      <c r="B73" s="375"/>
-      <c r="C73" s="379"/>
+      <c r="A73" s="412"/>
+      <c r="B73" s="418"/>
+      <c r="C73" s="422"/>
       <c r="D73" s="10" t="s">
         <v>17</v>
       </c>
@@ -5782,9 +5782,9 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="369"/>
-      <c r="B74" s="375"/>
-      <c r="C74" s="380"/>
+      <c r="A74" s="412"/>
+      <c r="B74" s="418"/>
+      <c r="C74" s="423"/>
       <c r="D74" s="10" t="s">
         <v>17</v>
       </c>
@@ -5808,8 +5808,8 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="369"/>
-      <c r="B75" s="375"/>
+      <c r="A75" s="412"/>
+      <c r="B75" s="418"/>
       <c r="C75" s="157" t="s">
         <v>210</v>
       </c>
@@ -5834,8 +5834,8 @@
       <c r="J75" s="277"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="369"/>
-      <c r="B76" s="376"/>
+      <c r="A76" s="412"/>
+      <c r="B76" s="419"/>
       <c r="C76" s="157" t="s">
         <v>211</v>
       </c>
@@ -5860,11 +5860,11 @@
       <c r="J76" s="277"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="369"/>
-      <c r="B77" s="373" t="s">
+      <c r="A77" s="412"/>
+      <c r="B77" s="416" t="s">
         <v>137</v>
       </c>
-      <c r="C77" s="360" t="s">
+      <c r="C77" s="406" t="s">
         <v>58</v>
       </c>
       <c r="D77" s="51" t="s">
@@ -5888,9 +5888,9 @@
       <c r="J77" s="273"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="369"/>
-      <c r="B78" s="374"/>
-      <c r="C78" s="361"/>
+      <c r="A78" s="412"/>
+      <c r="B78" s="417"/>
+      <c r="C78" s="407"/>
       <c r="D78" s="53" t="s">
         <v>17</v>
       </c>
@@ -5912,8 +5912,8 @@
       <c r="J78" s="275"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="369"/>
-      <c r="B79" s="374"/>
+      <c r="A79" s="412"/>
+      <c r="B79" s="417"/>
       <c r="C79" s="132" t="s">
         <v>214</v>
       </c>
@@ -5938,8 +5938,8 @@
       <c r="J79" s="278"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="369"/>
-      <c r="B80" s="377"/>
+      <c r="A80" s="412"/>
+      <c r="B80" s="420"/>
       <c r="C80" s="132" t="s">
         <v>215</v>
       </c>
@@ -5964,7 +5964,7 @@
       <c r="J80" s="279"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="369"/>
+      <c r="A81" s="412"/>
       <c r="B81" s="163" t="s">
         <v>138</v>
       </c>
@@ -5992,7 +5992,7 @@
       <c r="J81" s="278"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="369"/>
+      <c r="A82" s="412"/>
       <c r="B82" s="186" t="s">
         <v>156</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="J82" s="280"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="369"/>
+      <c r="A83" s="412"/>
       <c r="B83" s="163" t="s">
         <v>216</v>
       </c>
@@ -6048,7 +6048,7 @@
       <c r="J83" s="278"/>
     </row>
     <row r="84" spans="1:10" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="370"/>
+      <c r="A84" s="413"/>
       <c r="B84" s="162" t="s">
         <v>219</v>
       </c>
@@ -6076,7 +6076,7 @@
       <c r="J84" s="279"/>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="365" t="s">
+      <c r="A85" s="376" t="s">
         <v>140</v>
       </c>
       <c r="B85" s="187" t="s">
@@ -6106,8 +6106,8 @@
       <c r="J85" s="281"/>
     </row>
     <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="366"/>
-      <c r="B86" s="362" t="s">
+      <c r="A86" s="378"/>
+      <c r="B86" s="408" t="s">
         <v>181</v>
       </c>
       <c r="C86" s="36" t="s">
@@ -6134,8 +6134,8 @@
       <c r="J86" s="269"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="366"/>
-      <c r="B87" s="363"/>
+      <c r="A87" s="378"/>
+      <c r="B87" s="409"/>
       <c r="C87" s="36" t="s">
         <v>64</v>
       </c>
@@ -6160,8 +6160,8 @@
       <c r="J87" s="269"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="366"/>
-      <c r="B88" s="363"/>
+      <c r="A88" s="378"/>
+      <c r="B88" s="409"/>
       <c r="C88" s="36" t="s">
         <v>68</v>
       </c>
@@ -6188,8 +6188,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="366"/>
-      <c r="B89" s="364"/>
+      <c r="A89" s="378"/>
+      <c r="B89" s="410"/>
       <c r="C89" s="36" t="s">
         <v>69</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="367"/>
+      <c r="A90" s="377"/>
       <c r="B90" s="188" t="s">
         <v>182</v>
       </c>
@@ -6245,10 +6245,10 @@
     </row>
     <row r="91" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="328"/>
-      <c r="B91" s="415" t="s">
+      <c r="B91" s="358" t="s">
         <v>141</v>
       </c>
-      <c r="C91" s="398" t="s">
+      <c r="C91" s="393" t="s">
         <v>71</v>
       </c>
       <c r="D91" s="17" t="s">
@@ -6274,9 +6274,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="83" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="413"/>
-      <c r="B92" s="416"/>
-      <c r="C92" s="399"/>
+      <c r="A92" s="356"/>
+      <c r="B92" s="359"/>
+      <c r="C92" s="394"/>
       <c r="D92" s="71" t="s">
         <v>17</v>
       </c>
@@ -6298,7 +6298,7 @@
       <c r="J92" s="282"/>
     </row>
     <row r="93" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="413"/>
+      <c r="A93" s="356"/>
       <c r="B93" s="189" t="s">
         <v>142</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="J93" s="283"/>
     </row>
     <row r="94" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="413"/>
+      <c r="A94" s="356"/>
       <c r="B94" s="190" t="s">
         <v>143</v>
       </c>
@@ -6354,7 +6354,7 @@
       <c r="J94" s="283"/>
     </row>
     <row r="95" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="413"/>
+      <c r="A95" s="356"/>
       <c r="B95" s="190" t="s">
         <v>144</v>
       </c>
@@ -6382,7 +6382,7 @@
       <c r="J95" s="283"/>
     </row>
     <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="414"/>
+      <c r="A96" s="357"/>
       <c r="B96" s="190" t="s">
         <v>145</v>
       </c>
@@ -6412,7 +6412,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="365" t="s">
+      <c r="A97" s="376" t="s">
         <v>146</v>
       </c>
       <c r="B97" s="191" t="s">
@@ -6442,7 +6442,7 @@
       <c r="J97" s="269"/>
     </row>
     <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="367"/>
+      <c r="A98" s="377"/>
       <c r="B98" s="192" t="s">
         <v>148</v>
       </c>
@@ -6472,10 +6472,10 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="395" t="s">
+      <c r="A99" s="390" t="s">
         <v>151</v>
       </c>
-      <c r="B99" s="384" t="s">
+      <c r="B99" s="427" t="s">
         <v>149</v>
       </c>
       <c r="C99" s="43" t="s">
@@ -6502,8 +6502,8 @@
       <c r="J99" s="286"/>
     </row>
     <row r="100" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="396"/>
-      <c r="B100" s="385"/>
+      <c r="A100" s="391"/>
+      <c r="B100" s="428"/>
       <c r="C100" s="45" t="s">
         <v>83</v>
       </c>
@@ -6530,7 +6530,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="397"/>
+      <c r="A101" s="392"/>
       <c r="B101" s="193" t="s">
         <v>150</v>
       </c>
@@ -6558,11 +6558,11 @@
       <c r="J101" s="288"/>
     </row>
     <row r="102" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="365" t="s">
+      <c r="A102" s="376" t="s">
         <v>152</v>
       </c>
       <c r="B102" s="194"/>
-      <c r="C102" s="353" t="s">
+      <c r="C102" s="400" t="s">
         <v>85</v>
       </c>
       <c r="D102" s="33" t="s">
@@ -6586,9 +6586,9 @@
       <c r="J102" s="289"/>
     </row>
     <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="366"/>
+      <c r="A103" s="378"/>
       <c r="B103" s="195"/>
-      <c r="C103" s="354"/>
+      <c r="C103" s="401"/>
       <c r="D103" s="35" t="s">
         <v>17</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="367"/>
+      <c r="A104" s="377"/>
       <c r="B104" s="196"/>
       <c r="C104" s="15" t="s">
         <v>86</v>
@@ -6640,7 +6640,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="386" t="s">
+      <c r="A105" s="383" t="s">
         <v>153</v>
       </c>
       <c r="B105" s="197" t="s">
@@ -6670,7 +6670,7 @@
       <c r="J105" s="292"/>
     </row>
     <row r="106" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="387"/>
+      <c r="A106" s="384"/>
       <c r="B106" s="197" t="s">
         <v>155</v>
       </c>
@@ -6698,7 +6698,7 @@
       <c r="J106" s="293"/>
     </row>
     <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="388"/>
+      <c r="A107" s="385"/>
       <c r="B107" s="197" t="s">
         <v>154</v>
       </c>
@@ -6726,7 +6726,7 @@
       <c r="J107" s="294"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="355" t="s">
+      <c r="A108" s="382" t="s">
         <v>159</v>
       </c>
       <c r="B108" s="198" t="s">
@@ -6756,7 +6756,7 @@
       <c r="J108" s="269"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="356"/>
+      <c r="A109" s="402"/>
       <c r="B109" s="199" t="s">
         <v>158</v>
       </c>
@@ -6786,7 +6786,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="357"/>
+      <c r="A110" s="403"/>
       <c r="B110" s="200" t="s">
         <v>206</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="J110" s="291"/>
     </row>
     <row r="111" spans="1:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="371" t="s">
+      <c r="A111" s="414" t="s">
         <v>160</v>
       </c>
       <c r="B111" s="201" t="s">
@@ -6844,7 +6844,7 @@
       <c r="J111" s="296"/>
     </row>
     <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="372"/>
+      <c r="A112" s="415"/>
       <c r="B112" s="202" t="s">
         <v>162</v>
       </c>
@@ -6872,7 +6872,7 @@
       <c r="J112" s="297"/>
     </row>
     <row r="113" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="365" t="s">
+      <c r="A113" s="376" t="s">
         <v>163</v>
       </c>
       <c r="B113" s="203" t="s">
@@ -6902,7 +6902,7 @@
       <c r="J113" s="272"/>
     </row>
     <row r="114" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="366"/>
+      <c r="A114" s="378"/>
       <c r="B114" s="204" t="s">
         <v>104</v>
       </c>
@@ -6932,7 +6932,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="367"/>
+      <c r="A115" s="377"/>
       <c r="B115" s="205" t="s">
         <v>113</v>
       </c>
@@ -6962,7 +6962,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="355" t="s">
+      <c r="A116" s="382" t="s">
         <v>207</v>
       </c>
       <c r="B116" s="206" t="s">
@@ -6992,7 +6992,7 @@
       <c r="J116" s="269"/>
     </row>
     <row r="117" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="367"/>
+      <c r="A117" s="377"/>
       <c r="B117" s="207" t="s">
         <v>208</v>
       </c>
@@ -7020,7 +7020,7 @@
       <c r="J117" s="285"/>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="365" t="s">
+      <c r="A118" s="376" t="s">
         <v>233</v>
       </c>
       <c r="B118" s="185" t="s">
@@ -7050,7 +7050,7 @@
       <c r="J118" s="298"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="367"/>
+      <c r="A119" s="377"/>
       <c r="B119" s="207" t="s">
         <v>234</v>
       </c>
@@ -7108,7 +7108,7 @@
       <c r="J120" s="299"/>
     </row>
     <row r="121" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="365" t="s">
+      <c r="A121" s="376" t="s">
         <v>167</v>
       </c>
       <c r="B121" s="185" t="s">
@@ -7140,7 +7140,7 @@
       </c>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="367"/>
+      <c r="A122" s="377"/>
       <c r="B122" s="207" t="s">
         <v>173</v>
       </c>
@@ -7386,11 +7386,11 @@
       <c r="J129" s="272"/>
     </row>
     <row r="130" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="350" t="s">
+      <c r="A130" s="397" t="s">
         <v>178</v>
       </c>
       <c r="B130" s="210"/>
-      <c r="C130" s="381" t="s">
+      <c r="C130" s="424" t="s">
         <v>125</v>
       </c>
       <c r="D130" s="86" t="s">
@@ -7416,9 +7416,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="351"/>
+      <c r="A131" s="398"/>
       <c r="B131" s="210"/>
-      <c r="C131" s="382"/>
+      <c r="C131" s="425"/>
       <c r="D131" s="88" t="s">
         <v>17</v>
       </c>
@@ -7442,9 +7442,9 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="351"/>
+      <c r="A132" s="398"/>
       <c r="B132" s="210"/>
-      <c r="C132" s="382"/>
+      <c r="C132" s="425"/>
       <c r="D132" s="91" t="s">
         <v>17</v>
       </c>
@@ -7468,9 +7468,9 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="351"/>
+      <c r="A133" s="398"/>
       <c r="B133" s="211"/>
-      <c r="C133" s="382"/>
+      <c r="C133" s="425"/>
       <c r="D133" s="91" t="s">
         <v>17</v>
       </c>
@@ -7494,9 +7494,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="351"/>
+      <c r="A134" s="398"/>
       <c r="B134" s="212"/>
-      <c r="C134" s="383"/>
+      <c r="C134" s="426"/>
       <c r="D134" s="92" t="s">
         <v>17</v>
       </c>
@@ -7520,9 +7520,9 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="351"/>
+      <c r="A135" s="398"/>
       <c r="B135" s="212"/>
-      <c r="C135" s="348" t="s">
+      <c r="C135" s="395" t="s">
         <v>129</v>
       </c>
       <c r="D135" s="94" t="s">
@@ -7548,9 +7548,9 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="351"/>
+      <c r="A136" s="398"/>
       <c r="B136" s="212"/>
-      <c r="C136" s="349"/>
+      <c r="C136" s="396"/>
       <c r="D136" s="96" t="s">
         <v>17</v>
       </c>
@@ -7574,7 +7574,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="352"/>
+      <c r="A137" s="399"/>
       <c r="B137" s="213"/>
       <c r="C137" s="147" t="s">
         <v>131</v>
@@ -7602,7 +7602,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="402" t="s">
+      <c r="A138" s="379" t="s">
         <v>186</v>
       </c>
       <c r="B138" s="214"/>
@@ -7630,7 +7630,7 @@
       <c r="J138" s="306"/>
     </row>
     <row r="139" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A139" s="403"/>
+      <c r="A139" s="380"/>
       <c r="B139" s="215"/>
       <c r="C139" s="2" t="s">
         <v>188</v>
@@ -7656,7 +7656,7 @@
       <c r="J139" s="307"/>
     </row>
     <row r="140" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="404"/>
+      <c r="A140" s="381"/>
       <c r="B140" s="216"/>
       <c r="C140" s="20" t="s">
         <v>244</v>
@@ -7682,7 +7682,7 @@
       <c r="J140" s="308"/>
     </row>
     <row r="141" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A141" s="402" t="s">
+      <c r="A141" s="379" t="s">
         <v>192</v>
       </c>
       <c r="B141" s="214"/>
@@ -7710,7 +7710,7 @@
       <c r="J141" s="306"/>
     </row>
     <row r="142" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="403"/>
+      <c r="A142" s="380"/>
       <c r="B142" s="215"/>
       <c r="C142" s="329" t="s">
         <v>395</v>
@@ -7736,7 +7736,7 @@
       <c r="J142" s="307"/>
     </row>
     <row r="143" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="404"/>
+      <c r="A143" s="381"/>
       <c r="B143" s="217"/>
       <c r="C143" s="329" t="s">
         <v>396</v>
@@ -7846,7 +7846,7 @@
       <c r="J146" s="311"/>
     </row>
     <row r="147" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="400" t="s">
+      <c r="A147" s="374" t="s">
         <v>223</v>
       </c>
       <c r="B147" s="220" t="s">
@@ -7876,7 +7876,7 @@
       <c r="J147" s="312"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="401"/>
+      <c r="A148" s="375"/>
       <c r="B148" s="221" t="s">
         <v>248</v>
       </c>
@@ -9145,36 +9145,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="B28:B46"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B12:B27"/>
-    <mergeCell ref="A28:A51"/>
-    <mergeCell ref="C28:C41"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="C91:C92"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="C102:C103"/>
@@ -9191,6 +9161,36 @@
     <mergeCell ref="C130:C134"/>
     <mergeCell ref="A97:A98"/>
     <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="B28:B46"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B12:B27"/>
+    <mergeCell ref="A28:A51"/>
+    <mergeCell ref="C28:C41"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C12:C23"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9202,8 +9202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADEA23E-E81E-4AF5-920B-9A516112A0D6}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9829,7 +9829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0549DD8A-C168-4BC3-BE80-FD94021F7EEB}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first step of following bartools vignette and clean up of renv packages
</commit_message>
<xml_diff>
--- a/data/Table of compounds_whole_2025-06-13.xlsx
+++ b/data/Table of compounds_whole_2025-06-13.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="356" documentId="13_ncr:1_{4AEB09D8-4E79-4CE5-B440-217971482316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A217C753-7B86-42BA-9E4F-4E4FFAC8CA47}"/>
+  <xr:revisionPtr revIDLastSave="360" documentId="13_ncr:1_{4AEB09D8-4E79-4CE5-B440-217971482316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99E0E2DE-9614-4026-94AF-9BD7FC9C221E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4240" yWindow="0" windowWidth="9780" windowHeight="10800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Design" sheetId="2" r:id="rId1"/>
@@ -1228,9 +1228,6 @@
     <t>5uM concentration was not enough to kill the cells</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>0d</t>
   </si>
   <si>
@@ -1556,6 +1553,9 @@
       </rPr>
       <t xml:space="preserve"> Does not contain controls, so merged with exp200921!!</t>
     </r>
+  </si>
+  <si>
+    <t>000 uM</t>
   </si>
 </sst>
 </file>
@@ -3206,6 +3206,177 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3242,12 +3413,6 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3283,171 +3448,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3852,11 +3852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J271"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3903,20 +3903,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="348" t="s">
+      <c r="A2" s="405" t="s">
         <v>372</v>
       </c>
-      <c r="B2" s="348" t="s">
+      <c r="B2" s="405" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="348" t="s">
+      <c r="C2" s="405" t="s">
         <v>372</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
@@ -3925,7 +3925,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>346</v>
@@ -3933,14 +3933,14 @@
       <c r="J2" s="320"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="349"/>
-      <c r="B3" s="349"/>
-      <c r="C3" s="349"/>
+      <c r="A3" s="406"/>
+      <c r="B3" s="406"/>
+      <c r="C3" s="406"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
@@ -3949,7 +3949,7 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>346</v>
@@ -3957,14 +3957,14 @@
       <c r="J3" s="321"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="349"/>
-      <c r="B4" s="349"/>
-      <c r="C4" s="349"/>
+      <c r="A4" s="406"/>
+      <c r="B4" s="406"/>
+      <c r="C4" s="406"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>8</v>
@@ -3973,7 +3973,7 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>346</v>
@@ -3981,14 +3981,14 @@
       <c r="J4" s="321"/>
     </row>
     <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="349"/>
-      <c r="B5" s="349"/>
-      <c r="C5" s="349"/>
+      <c r="A5" s="406"/>
+      <c r="B5" s="406"/>
+      <c r="C5" s="406"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>8</v>
@@ -3997,7 +3997,7 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>346</v>
@@ -4007,14 +4007,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="349"/>
-      <c r="B6" s="349"/>
-      <c r="C6" s="349"/>
+      <c r="A6" s="406"/>
+      <c r="B6" s="406"/>
+      <c r="C6" s="406"/>
       <c r="D6" s="5" t="s">
         <v>373</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
@@ -4023,7 +4023,7 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>346</v>
@@ -4031,14 +4031,14 @@
       <c r="J6" s="321"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="349"/>
-      <c r="B7" s="349"/>
-      <c r="C7" s="349"/>
+      <c r="A7" s="406"/>
+      <c r="B7" s="406"/>
+      <c r="C7" s="406"/>
       <c r="D7" s="5" t="s">
         <v>373</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
@@ -4047,7 +4047,7 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>346</v>
@@ -4055,23 +4055,23 @@
       <c r="J7" s="321"/>
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="349"/>
-      <c r="B8" s="349"/>
-      <c r="C8" s="349"/>
+      <c r="A8" s="406"/>
+      <c r="B8" s="406"/>
+      <c r="C8" s="406"/>
       <c r="D8" s="322" t="s">
         <v>373</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="335" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>346</v>
@@ -4081,23 +4081,23 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="349"/>
-      <c r="B9" s="349"/>
-      <c r="C9" s="349"/>
+      <c r="A9" s="406"/>
+      <c r="B9" s="406"/>
+      <c r="C9" s="406"/>
       <c r="D9" t="s">
         <v>373</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="336" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>346</v>
@@ -4107,14 +4107,14 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="349"/>
-      <c r="B10" s="349"/>
-      <c r="C10" s="349"/>
+      <c r="A10" s="406"/>
+      <c r="B10" s="406"/>
+      <c r="C10" s="406"/>
       <c r="D10" s="323" t="s">
         <v>373</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F10" s="324" t="s">
         <v>184</v>
@@ -4123,7 +4123,7 @@
         <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>346</v>
@@ -4131,14 +4131,14 @@
       <c r="J10" s="325"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="350"/>
-      <c r="B11" s="350"/>
-      <c r="C11" s="350"/>
+      <c r="A11" s="407"/>
+      <c r="B11" s="407"/>
+      <c r="C11" s="407"/>
       <c r="D11" s="326" t="s">
         <v>373</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F11" s="326" t="s">
         <v>213</v>
@@ -4147,7 +4147,7 @@
         <v>237</v>
       </c>
       <c r="H11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>346</v>
@@ -4155,20 +4155,20 @@
       <c r="J11" s="327"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="351" t="s">
+      <c r="A12" s="408" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="351" t="s">
+      <c r="B12" s="408" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="348" t="s">
+      <c r="C12" s="405" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
@@ -4185,14 +4185,14 @@
       <c r="J12" s="247"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="352"/>
-      <c r="B13" s="352"/>
-      <c r="C13" s="373"/>
+      <c r="A13" s="409"/>
+      <c r="B13" s="409"/>
+      <c r="C13" s="428"/>
       <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -4208,14 +4208,14 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="352"/>
-      <c r="B14" s="352"/>
-      <c r="C14" s="373"/>
+      <c r="A14" s="409"/>
+      <c r="B14" s="409"/>
+      <c r="C14" s="428"/>
       <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
@@ -4232,14 +4232,14 @@
       <c r="J14" s="248"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="352"/>
-      <c r="B15" s="352"/>
-      <c r="C15" s="373"/>
+      <c r="A15" s="409"/>
+      <c r="B15" s="409"/>
+      <c r="C15" s="428"/>
       <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>20</v>
@@ -4256,14 +4256,14 @@
       <c r="J15" s="248"/>
     </row>
     <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="352"/>
-      <c r="B16" s="352"/>
-      <c r="C16" s="373"/>
+      <c r="A16" s="409"/>
+      <c r="B16" s="409"/>
+      <c r="C16" s="428"/>
       <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>8</v>
@@ -4280,14 +4280,14 @@
       <c r="J16" s="248"/>
     </row>
     <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="352"/>
-      <c r="B17" s="352"/>
-      <c r="C17" s="373"/>
+      <c r="A17" s="409"/>
+      <c r="B17" s="409"/>
+      <c r="C17" s="428"/>
       <c r="D17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
@@ -4306,14 +4306,14 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="352"/>
-      <c r="B18" s="352"/>
-      <c r="C18" s="373"/>
+      <c r="A18" s="409"/>
+      <c r="B18" s="409"/>
+      <c r="C18" s="428"/>
       <c r="D18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>14</v>
@@ -4330,20 +4330,20 @@
       <c r="J18" s="250"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="352"/>
-      <c r="B19" s="352"/>
-      <c r="C19" s="373"/>
+      <c r="A19" s="409"/>
+      <c r="B19" s="409"/>
+      <c r="C19" s="428"/>
       <c r="D19" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="336" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H19" t="s">
         <v>349</v>
@@ -4354,14 +4354,14 @@
       <c r="J19" s="251"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="352"/>
-      <c r="B20" s="352"/>
-      <c r="C20" s="373"/>
+      <c r="A20" s="409"/>
+      <c r="B20" s="409"/>
+      <c r="C20" s="428"/>
       <c r="D20" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>184</v>
@@ -4378,14 +4378,14 @@
       <c r="J20" s="252"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="352"/>
-      <c r="B21" s="352"/>
-      <c r="C21" s="373"/>
+      <c r="A21" s="409"/>
+      <c r="B21" s="409"/>
+      <c r="C21" s="428"/>
       <c r="D21" s="113" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F21" s="113" t="s">
         <v>213</v>
@@ -4402,14 +4402,14 @@
       <c r="J21" s="253"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="352"/>
-      <c r="B22" s="352"/>
-      <c r="C22" s="373"/>
+      <c r="A22" s="409"/>
+      <c r="B22" s="409"/>
+      <c r="C22" s="428"/>
       <c r="D22" s="98" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F22" s="98" t="s">
         <v>8</v>
@@ -4428,14 +4428,14 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="352"/>
-      <c r="B23" s="352"/>
-      <c r="C23" s="373"/>
+      <c r="A23" s="409"/>
+      <c r="B23" s="409"/>
+      <c r="C23" s="428"/>
       <c r="D23" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>336</v>
@@ -4452,16 +4452,16 @@
       <c r="J23" s="252"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="352"/>
-      <c r="B24" s="352"/>
+      <c r="A24" s="409"/>
+      <c r="B24" s="409"/>
       <c r="C24" s="331" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D24" s="172" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>336</v>
@@ -4480,16 +4480,16 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="352"/>
-      <c r="B25" s="352"/>
+      <c r="A25" s="409"/>
+      <c r="B25" s="409"/>
       <c r="C25" s="331" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D25" s="172" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>336</v>
@@ -4508,16 +4508,16 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="352"/>
-      <c r="B26" s="352"/>
+      <c r="A26" s="409"/>
+      <c r="B26" s="409"/>
       <c r="C26" s="331" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D26" s="172" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>336</v>
@@ -4536,8 +4536,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="352"/>
-      <c r="B27" s="352"/>
+      <c r="A27" s="409"/>
+      <c r="B27" s="409"/>
       <c r="C27" s="331" t="s">
         <v>16</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="F27" s="172" t="s">
         <v>336</v>
@@ -4564,13 +4564,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="362" t="s">
+      <c r="A28" s="417" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="353" t="s">
+      <c r="B28" s="410" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="365" t="s">
+      <c r="C28" s="420" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="99" t="s">
@@ -4596,9 +4596,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="363"/>
-      <c r="B29" s="354"/>
-      <c r="C29" s="366"/>
+      <c r="A29" s="418"/>
+      <c r="B29" s="411"/>
+      <c r="C29" s="421"/>
       <c r="D29" s="100" t="s">
         <v>17</v>
       </c>
@@ -4620,9 +4620,9 @@
       <c r="J29" s="257"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="363"/>
-      <c r="B30" s="354"/>
-      <c r="C30" s="366"/>
+      <c r="A30" s="418"/>
+      <c r="B30" s="411"/>
+      <c r="C30" s="421"/>
       <c r="D30" s="102" t="s">
         <v>17</v>
       </c>
@@ -4644,9 +4644,9 @@
       <c r="J30" s="249"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="363"/>
-      <c r="B31" s="354"/>
-      <c r="C31" s="366"/>
+      <c r="A31" s="418"/>
+      <c r="B31" s="411"/>
+      <c r="C31" s="421"/>
       <c r="D31" s="102" t="s">
         <v>17</v>
       </c>
@@ -4668,9 +4668,9 @@
       <c r="J31" s="249"/>
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="363"/>
-      <c r="B32" s="354"/>
-      <c r="C32" s="366"/>
+      <c r="A32" s="418"/>
+      <c r="B32" s="411"/>
+      <c r="C32" s="421"/>
       <c r="D32" s="102" t="s">
         <v>17</v>
       </c>
@@ -4694,9 +4694,9 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="363"/>
-      <c r="B33" s="354"/>
-      <c r="C33" s="366"/>
+      <c r="A33" s="418"/>
+      <c r="B33" s="411"/>
+      <c r="C33" s="421"/>
       <c r="D33" s="102" t="s">
         <v>17</v>
       </c>
@@ -4720,9 +4720,9 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="363"/>
-      <c r="B34" s="354"/>
-      <c r="C34" s="366"/>
+      <c r="A34" s="418"/>
+      <c r="B34" s="411"/>
+      <c r="C34" s="421"/>
       <c r="D34" s="102" t="s">
         <v>17</v>
       </c>
@@ -4746,9 +4746,9 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="363"/>
-      <c r="B35" s="354"/>
-      <c r="C35" s="366"/>
+      <c r="A35" s="418"/>
+      <c r="B35" s="411"/>
+      <c r="C35" s="421"/>
       <c r="D35" s="128" t="s">
         <v>17</v>
       </c>
@@ -4772,9 +4772,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="363"/>
-      <c r="B36" s="354"/>
-      <c r="C36" s="366"/>
+      <c r="A36" s="418"/>
+      <c r="B36" s="411"/>
+      <c r="C36" s="421"/>
       <c r="D36" s="128" t="s">
         <v>17</v>
       </c>
@@ -4798,9 +4798,9 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="363"/>
-      <c r="B37" s="354"/>
-      <c r="C37" s="366"/>
+      <c r="A37" s="418"/>
+      <c r="B37" s="411"/>
+      <c r="C37" s="421"/>
       <c r="D37" s="128" t="s">
         <v>17</v>
       </c>
@@ -4824,9 +4824,9 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="363"/>
-      <c r="B38" s="354"/>
-      <c r="C38" s="366"/>
+      <c r="A38" s="418"/>
+      <c r="B38" s="411"/>
+      <c r="C38" s="421"/>
       <c r="D38" s="128" t="s">
         <v>17</v>
       </c>
@@ -4850,9 +4850,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="363"/>
-      <c r="B39" s="354"/>
-      <c r="C39" s="366"/>
+      <c r="A39" s="418"/>
+      <c r="B39" s="411"/>
+      <c r="C39" s="421"/>
       <c r="D39" s="128" t="s">
         <v>17</v>
       </c>
@@ -4876,9 +4876,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="363"/>
-      <c r="B40" s="354"/>
-      <c r="C40" s="366"/>
+      <c r="A40" s="418"/>
+      <c r="B40" s="411"/>
+      <c r="C40" s="421"/>
       <c r="D40" s="128" t="s">
         <v>17</v>
       </c>
@@ -4902,9 +4902,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="363"/>
-      <c r="B41" s="354"/>
-      <c r="C41" s="367"/>
+      <c r="A41" s="418"/>
+      <c r="B41" s="411"/>
+      <c r="C41" s="422"/>
       <c r="D41" s="128" t="s">
         <v>17</v>
       </c>
@@ -4928,8 +4928,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="363"/>
-      <c r="B42" s="354"/>
+      <c r="A42" s="418"/>
+      <c r="B42" s="411"/>
       <c r="C42" s="110" t="s">
         <v>32</v>
       </c>
@@ -4956,8 +4956,8 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="363"/>
-      <c r="B43" s="354"/>
+      <c r="A43" s="418"/>
+      <c r="B43" s="411"/>
       <c r="C43" s="136" t="s">
         <v>197</v>
       </c>
@@ -4982,8 +4982,8 @@
       <c r="J43" s="259"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="363"/>
-      <c r="B44" s="354"/>
+      <c r="A44" s="418"/>
+      <c r="B44" s="411"/>
       <c r="C44" s="136" t="s">
         <v>198</v>
       </c>
@@ -5008,8 +5008,8 @@
       <c r="J44" s="259"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="363"/>
-      <c r="B45" s="354"/>
+      <c r="A45" s="418"/>
+      <c r="B45" s="411"/>
       <c r="C45" s="127" t="s">
         <v>199</v>
       </c>
@@ -5034,8 +5034,8 @@
       <c r="J45" s="260"/>
     </row>
     <row r="46" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="363"/>
-      <c r="B46" s="355"/>
+      <c r="A46" s="418"/>
+      <c r="B46" s="412"/>
       <c r="C46" s="174" t="s">
         <v>321</v>
       </c>
@@ -5062,11 +5062,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="363"/>
-      <c r="B47" s="370" t="s">
+      <c r="A47" s="418"/>
+      <c r="B47" s="425" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="371" t="s">
+      <c r="C47" s="426" t="s">
         <v>29</v>
       </c>
       <c r="D47" s="100" t="s">
@@ -5090,9 +5090,9 @@
       <c r="J47" s="257"/>
     </row>
     <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="363"/>
-      <c r="B48" s="368"/>
-      <c r="C48" s="371"/>
+      <c r="A48" s="418"/>
+      <c r="B48" s="423"/>
+      <c r="C48" s="426"/>
       <c r="D48" s="105" t="s">
         <v>17</v>
       </c>
@@ -5114,9 +5114,9 @@
       <c r="J48" s="261"/>
     </row>
     <row r="49" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="363"/>
-      <c r="B49" s="368"/>
-      <c r="C49" s="372"/>
+      <c r="A49" s="418"/>
+      <c r="B49" s="423"/>
+      <c r="C49" s="427"/>
       <c r="D49" s="173" t="s">
         <v>17</v>
       </c>
@@ -5140,8 +5140,8 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="363"/>
-      <c r="B50" s="368" t="s">
+      <c r="A50" s="418"/>
+      <c r="B50" s="423" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="130" t="s">
@@ -5168,8 +5168,8 @@
       <c r="J50" s="314"/>
     </row>
     <row r="51" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="364"/>
-      <c r="B51" s="369"/>
+      <c r="A51" s="419"/>
+      <c r="B51" s="424"/>
       <c r="C51" s="130" t="s">
         <v>132</v>
       </c>
@@ -5226,11 +5226,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="387" t="s">
+      <c r="A53" s="392" t="s">
         <v>35</v>
       </c>
       <c r="B53" s="178"/>
-      <c r="C53" s="360" t="s">
+      <c r="C53" s="389" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="57" t="s">
@@ -5254,9 +5254,9 @@
       <c r="J53" s="263"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="388"/>
+      <c r="A54" s="393"/>
       <c r="B54" s="178"/>
-      <c r="C54" s="361"/>
+      <c r="C54" s="390"/>
       <c r="D54" s="60" t="s">
         <v>17</v>
       </c>
@@ -5278,9 +5278,9 @@
       <c r="J54" s="264"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="388"/>
+      <c r="A55" s="393"/>
       <c r="B55" s="178"/>
-      <c r="C55" s="360" t="s">
+      <c r="C55" s="389" t="s">
         <v>36</v>
       </c>
       <c r="D55" s="57" t="s">
@@ -5304,9 +5304,9 @@
       <c r="J55" s="263"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="388"/>
+      <c r="A56" s="393"/>
       <c r="B56" s="178"/>
-      <c r="C56" s="361"/>
+      <c r="C56" s="390"/>
       <c r="D56" s="60" t="s">
         <v>17</v>
       </c>
@@ -5328,7 +5328,7 @@
       <c r="J56" s="264"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="388"/>
+      <c r="A57" s="393"/>
       <c r="B57" s="179"/>
       <c r="C57" s="143" t="s">
         <v>38</v>
@@ -5354,7 +5354,7 @@
       <c r="J57" s="265"/>
     </row>
     <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="389"/>
+      <c r="A58" s="394"/>
       <c r="B58" s="180"/>
       <c r="C58" s="64" t="s">
         <v>201</v>
@@ -5380,11 +5380,11 @@
       <c r="J58" s="266"/>
     </row>
     <row r="59" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="378" t="s">
+      <c r="A59" s="366" t="s">
         <v>43</v>
       </c>
       <c r="B59" s="181"/>
-      <c r="C59" s="386" t="s">
+      <c r="C59" s="391" t="s">
         <v>41</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5408,9 +5408,9 @@
       <c r="J59" s="267"/>
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="378"/>
+      <c r="A60" s="366"/>
       <c r="B60" s="181"/>
-      <c r="C60" s="386"/>
+      <c r="C60" s="391"/>
       <c r="D60" s="5" t="s">
         <v>17</v>
       </c>
@@ -5432,9 +5432,9 @@
       <c r="J60" s="248"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="378"/>
+      <c r="A61" s="366"/>
       <c r="B61" s="181"/>
-      <c r="C61" s="386"/>
+      <c r="C61" s="391"/>
       <c r="D61" s="8" t="s">
         <v>17</v>
       </c>
@@ -5456,7 +5456,7 @@
       <c r="J61" s="268"/>
     </row>
     <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="377"/>
+      <c r="A62" s="367"/>
       <c r="B62" s="182"/>
       <c r="C62" s="30" t="s">
         <v>45</v>
@@ -5482,7 +5482,7 @@
       <c r="J62" s="269"/>
     </row>
     <row r="63" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="404" t="s">
+      <c r="A63" s="358" t="s">
         <v>50</v>
       </c>
       <c r="B63" s="183" t="s">
@@ -5514,7 +5514,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="405"/>
+      <c r="A64" s="359"/>
       <c r="B64" s="184" t="s">
         <v>50</v>
       </c>
@@ -5574,13 +5574,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="411" t="s">
+      <c r="A66" s="368" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="416" t="s">
+      <c r="B66" s="373" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="421" t="s">
+      <c r="C66" s="378" t="s">
         <v>54</v>
       </c>
       <c r="D66" s="51" t="s">
@@ -5604,9 +5604,9 @@
       <c r="J66" s="273"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="412"/>
-      <c r="B67" s="417"/>
-      <c r="C67" s="422"/>
+      <c r="A67" s="369"/>
+      <c r="B67" s="374"/>
+      <c r="C67" s="379"/>
       <c r="D67" s="40" t="s">
         <v>17</v>
       </c>
@@ -5628,9 +5628,9 @@
       <c r="J67" s="274"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="412"/>
-      <c r="B68" s="417"/>
-      <c r="C68" s="422"/>
+      <c r="A68" s="369"/>
+      <c r="B68" s="374"/>
+      <c r="C68" s="379"/>
       <c r="D68" s="53" t="s">
         <v>17</v>
       </c>
@@ -5652,9 +5652,9 @@
       <c r="J68" s="275"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="412"/>
-      <c r="B69" s="418"/>
-      <c r="C69" s="422"/>
+      <c r="A69" s="369"/>
+      <c r="B69" s="375"/>
+      <c r="C69" s="379"/>
       <c r="D69" s="10" t="s">
         <v>17</v>
       </c>
@@ -5678,9 +5678,9 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="412"/>
-      <c r="B70" s="418"/>
-      <c r="C70" s="422"/>
+      <c r="A70" s="369"/>
+      <c r="B70" s="375"/>
+      <c r="C70" s="379"/>
       <c r="D70" s="10" t="s">
         <v>17</v>
       </c>
@@ -5704,9 +5704,9 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="412"/>
-      <c r="B71" s="418"/>
-      <c r="C71" s="422"/>
+      <c r="A71" s="369"/>
+      <c r="B71" s="375"/>
+      <c r="C71" s="379"/>
       <c r="D71" s="10" t="s">
         <v>17</v>
       </c>
@@ -5730,9 +5730,9 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="412"/>
-      <c r="B72" s="418"/>
-      <c r="C72" s="422"/>
+      <c r="A72" s="369"/>
+      <c r="B72" s="375"/>
+      <c r="C72" s="379"/>
       <c r="D72" s="10" t="s">
         <v>17</v>
       </c>
@@ -5756,9 +5756,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="412"/>
-      <c r="B73" s="418"/>
-      <c r="C73" s="422"/>
+      <c r="A73" s="369"/>
+      <c r="B73" s="375"/>
+      <c r="C73" s="379"/>
       <c r="D73" s="10" t="s">
         <v>17</v>
       </c>
@@ -5782,9 +5782,9 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="412"/>
-      <c r="B74" s="418"/>
-      <c r="C74" s="423"/>
+      <c r="A74" s="369"/>
+      <c r="B74" s="375"/>
+      <c r="C74" s="380"/>
       <c r="D74" s="10" t="s">
         <v>17</v>
       </c>
@@ -5808,8 +5808,8 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="412"/>
-      <c r="B75" s="418"/>
+      <c r="A75" s="369"/>
+      <c r="B75" s="375"/>
       <c r="C75" s="157" t="s">
         <v>210</v>
       </c>
@@ -5834,8 +5834,8 @@
       <c r="J75" s="277"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="412"/>
-      <c r="B76" s="419"/>
+      <c r="A76" s="369"/>
+      <c r="B76" s="376"/>
       <c r="C76" s="157" t="s">
         <v>211</v>
       </c>
@@ -5860,11 +5860,11 @@
       <c r="J76" s="277"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="412"/>
-      <c r="B77" s="416" t="s">
+      <c r="A77" s="369"/>
+      <c r="B77" s="373" t="s">
         <v>137</v>
       </c>
-      <c r="C77" s="406" t="s">
+      <c r="C77" s="360" t="s">
         <v>58</v>
       </c>
       <c r="D77" s="51" t="s">
@@ -5888,9 +5888,9 @@
       <c r="J77" s="273"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="412"/>
-      <c r="B78" s="417"/>
-      <c r="C78" s="407"/>
+      <c r="A78" s="369"/>
+      <c r="B78" s="374"/>
+      <c r="C78" s="361"/>
       <c r="D78" s="53" t="s">
         <v>17</v>
       </c>
@@ -5912,8 +5912,8 @@
       <c r="J78" s="275"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="412"/>
-      <c r="B79" s="417"/>
+      <c r="A79" s="369"/>
+      <c r="B79" s="374"/>
       <c r="C79" s="132" t="s">
         <v>214</v>
       </c>
@@ -5938,8 +5938,8 @@
       <c r="J79" s="278"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="412"/>
-      <c r="B80" s="420"/>
+      <c r="A80" s="369"/>
+      <c r="B80" s="377"/>
       <c r="C80" s="132" t="s">
         <v>215</v>
       </c>
@@ -5964,7 +5964,7 @@
       <c r="J80" s="279"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="412"/>
+      <c r="A81" s="369"/>
       <c r="B81" s="163" t="s">
         <v>138</v>
       </c>
@@ -5992,7 +5992,7 @@
       <c r="J81" s="278"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="412"/>
+      <c r="A82" s="369"/>
       <c r="B82" s="186" t="s">
         <v>156</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="J82" s="280"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="412"/>
+      <c r="A83" s="369"/>
       <c r="B83" s="163" t="s">
         <v>216</v>
       </c>
@@ -6048,7 +6048,7 @@
       <c r="J83" s="278"/>
     </row>
     <row r="84" spans="1:10" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="413"/>
+      <c r="A84" s="370"/>
       <c r="B84" s="162" t="s">
         <v>219</v>
       </c>
@@ -6076,7 +6076,7 @@
       <c r="J84" s="279"/>
     </row>
     <row r="85" spans="1:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="376" t="s">
+      <c r="A85" s="365" t="s">
         <v>140</v>
       </c>
       <c r="B85" s="187" t="s">
@@ -6106,8 +6106,8 @@
       <c r="J85" s="281"/>
     </row>
     <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="378"/>
-      <c r="B86" s="408" t="s">
+      <c r="A86" s="366"/>
+      <c r="B86" s="362" t="s">
         <v>181</v>
       </c>
       <c r="C86" s="36" t="s">
@@ -6134,8 +6134,8 @@
       <c r="J86" s="269"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="378"/>
-      <c r="B87" s="409"/>
+      <c r="A87" s="366"/>
+      <c r="B87" s="363"/>
       <c r="C87" s="36" t="s">
         <v>64</v>
       </c>
@@ -6160,8 +6160,8 @@
       <c r="J87" s="269"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="378"/>
-      <c r="B88" s="409"/>
+      <c r="A88" s="366"/>
+      <c r="B88" s="363"/>
       <c r="C88" s="36" t="s">
         <v>68</v>
       </c>
@@ -6188,8 +6188,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="378"/>
-      <c r="B89" s="410"/>
+      <c r="A89" s="366"/>
+      <c r="B89" s="364"/>
       <c r="C89" s="36" t="s">
         <v>69</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="377"/>
+      <c r="A90" s="367"/>
       <c r="B90" s="188" t="s">
         <v>182</v>
       </c>
@@ -6245,10 +6245,10 @@
     </row>
     <row r="91" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="328"/>
-      <c r="B91" s="358" t="s">
+      <c r="B91" s="415" t="s">
         <v>141</v>
       </c>
-      <c r="C91" s="393" t="s">
+      <c r="C91" s="398" t="s">
         <v>71</v>
       </c>
       <c r="D91" s="17" t="s">
@@ -6274,9 +6274,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="83" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="356"/>
-      <c r="B92" s="359"/>
-      <c r="C92" s="394"/>
+      <c r="A92" s="413"/>
+      <c r="B92" s="416"/>
+      <c r="C92" s="399"/>
       <c r="D92" s="71" t="s">
         <v>17</v>
       </c>
@@ -6298,7 +6298,7 @@
       <c r="J92" s="282"/>
     </row>
     <row r="93" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="356"/>
+      <c r="A93" s="413"/>
       <c r="B93" s="189" t="s">
         <v>142</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="J93" s="283"/>
     </row>
     <row r="94" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="356"/>
+      <c r="A94" s="413"/>
       <c r="B94" s="190" t="s">
         <v>143</v>
       </c>
@@ -6354,7 +6354,7 @@
       <c r="J94" s="283"/>
     </row>
     <row r="95" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="356"/>
+      <c r="A95" s="413"/>
       <c r="B95" s="190" t="s">
         <v>144</v>
       </c>
@@ -6382,7 +6382,7 @@
       <c r="J95" s="283"/>
     </row>
     <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="357"/>
+      <c r="A96" s="414"/>
       <c r="B96" s="190" t="s">
         <v>145</v>
       </c>
@@ -6412,7 +6412,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="376" t="s">
+      <c r="A97" s="365" t="s">
         <v>146</v>
       </c>
       <c r="B97" s="191" t="s">
@@ -6442,7 +6442,7 @@
       <c r="J97" s="269"/>
     </row>
     <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="377"/>
+      <c r="A98" s="367"/>
       <c r="B98" s="192" t="s">
         <v>148</v>
       </c>
@@ -6472,10 +6472,10 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="390" t="s">
+      <c r="A99" s="395" t="s">
         <v>151</v>
       </c>
-      <c r="B99" s="427" t="s">
+      <c r="B99" s="384" t="s">
         <v>149</v>
       </c>
       <c r="C99" s="43" t="s">
@@ -6502,8 +6502,8 @@
       <c r="J99" s="286"/>
     </row>
     <row r="100" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="391"/>
-      <c r="B100" s="428"/>
+      <c r="A100" s="396"/>
+      <c r="B100" s="385"/>
       <c r="C100" s="45" t="s">
         <v>83</v>
       </c>
@@ -6530,7 +6530,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="392"/>
+      <c r="A101" s="397"/>
       <c r="B101" s="193" t="s">
         <v>150</v>
       </c>
@@ -6558,11 +6558,11 @@
       <c r="J101" s="288"/>
     </row>
     <row r="102" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="376" t="s">
+      <c r="A102" s="365" t="s">
         <v>152</v>
       </c>
       <c r="B102" s="194"/>
-      <c r="C102" s="400" t="s">
+      <c r="C102" s="353" t="s">
         <v>85</v>
       </c>
       <c r="D102" s="33" t="s">
@@ -6586,9 +6586,9 @@
       <c r="J102" s="289"/>
     </row>
     <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="378"/>
+      <c r="A103" s="366"/>
       <c r="B103" s="195"/>
-      <c r="C103" s="401"/>
+      <c r="C103" s="354"/>
       <c r="D103" s="35" t="s">
         <v>17</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="377"/>
+      <c r="A104" s="367"/>
       <c r="B104" s="196"/>
       <c r="C104" s="15" t="s">
         <v>86</v>
@@ -6640,7 +6640,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="383" t="s">
+      <c r="A105" s="386" t="s">
         <v>153</v>
       </c>
       <c r="B105" s="197" t="s">
@@ -6670,7 +6670,7 @@
       <c r="J105" s="292"/>
     </row>
     <row r="106" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="384"/>
+      <c r="A106" s="387"/>
       <c r="B106" s="197" t="s">
         <v>155</v>
       </c>
@@ -6698,7 +6698,7 @@
       <c r="J106" s="293"/>
     </row>
     <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="385"/>
+      <c r="A107" s="388"/>
       <c r="B107" s="197" t="s">
         <v>154</v>
       </c>
@@ -6726,7 +6726,7 @@
       <c r="J107" s="294"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="382" t="s">
+      <c r="A108" s="355" t="s">
         <v>159</v>
       </c>
       <c r="B108" s="198" t="s">
@@ -6756,7 +6756,7 @@
       <c r="J108" s="269"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="402"/>
+      <c r="A109" s="356"/>
       <c r="B109" s="199" t="s">
         <v>158</v>
       </c>
@@ -6786,7 +6786,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="403"/>
+      <c r="A110" s="357"/>
       <c r="B110" s="200" t="s">
         <v>206</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="J110" s="291"/>
     </row>
     <row r="111" spans="1:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="414" t="s">
+      <c r="A111" s="371" t="s">
         <v>160</v>
       </c>
       <c r="B111" s="201" t="s">
@@ -6844,7 +6844,7 @@
       <c r="J111" s="296"/>
     </row>
     <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="415"/>
+      <c r="A112" s="372"/>
       <c r="B112" s="202" t="s">
         <v>162</v>
       </c>
@@ -6872,7 +6872,7 @@
       <c r="J112" s="297"/>
     </row>
     <row r="113" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="376" t="s">
+      <c r="A113" s="365" t="s">
         <v>163</v>
       </c>
       <c r="B113" s="203" t="s">
@@ -6902,7 +6902,7 @@
       <c r="J113" s="272"/>
     </row>
     <row r="114" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="378"/>
+      <c r="A114" s="366"/>
       <c r="B114" s="204" t="s">
         <v>104</v>
       </c>
@@ -6932,7 +6932,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="377"/>
+      <c r="A115" s="367"/>
       <c r="B115" s="205" t="s">
         <v>113</v>
       </c>
@@ -6962,7 +6962,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="382" t="s">
+      <c r="A116" s="355" t="s">
         <v>207</v>
       </c>
       <c r="B116" s="206" t="s">
@@ -6992,7 +6992,7 @@
       <c r="J116" s="269"/>
     </row>
     <row r="117" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="377"/>
+      <c r="A117" s="367"/>
       <c r="B117" s="207" t="s">
         <v>208</v>
       </c>
@@ -7020,7 +7020,7 @@
       <c r="J117" s="285"/>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="376" t="s">
+      <c r="A118" s="365" t="s">
         <v>233</v>
       </c>
       <c r="B118" s="185" t="s">
@@ -7050,7 +7050,7 @@
       <c r="J118" s="298"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="377"/>
+      <c r="A119" s="367"/>
       <c r="B119" s="207" t="s">
         <v>234</v>
       </c>
@@ -7108,7 +7108,7 @@
       <c r="J120" s="299"/>
     </row>
     <row r="121" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="376" t="s">
+      <c r="A121" s="365" t="s">
         <v>167</v>
       </c>
       <c r="B121" s="185" t="s">
@@ -7140,7 +7140,7 @@
       </c>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="377"/>
+      <c r="A122" s="367"/>
       <c r="B122" s="207" t="s">
         <v>173</v>
       </c>
@@ -7386,11 +7386,11 @@
       <c r="J129" s="272"/>
     </row>
     <row r="130" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="397" t="s">
+      <c r="A130" s="350" t="s">
         <v>178</v>
       </c>
       <c r="B130" s="210"/>
-      <c r="C130" s="424" t="s">
+      <c r="C130" s="381" t="s">
         <v>125</v>
       </c>
       <c r="D130" s="86" t="s">
@@ -7416,9 +7416,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="398"/>
+      <c r="A131" s="351"/>
       <c r="B131" s="210"/>
-      <c r="C131" s="425"/>
+      <c r="C131" s="382"/>
       <c r="D131" s="88" t="s">
         <v>17</v>
       </c>
@@ -7442,9 +7442,9 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="398"/>
+      <c r="A132" s="351"/>
       <c r="B132" s="210"/>
-      <c r="C132" s="425"/>
+      <c r="C132" s="382"/>
       <c r="D132" s="91" t="s">
         <v>17</v>
       </c>
@@ -7468,9 +7468,9 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="398"/>
+      <c r="A133" s="351"/>
       <c r="B133" s="211"/>
-      <c r="C133" s="425"/>
+      <c r="C133" s="382"/>
       <c r="D133" s="91" t="s">
         <v>17</v>
       </c>
@@ -7494,9 +7494,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="398"/>
+      <c r="A134" s="351"/>
       <c r="B134" s="212"/>
-      <c r="C134" s="426"/>
+      <c r="C134" s="383"/>
       <c r="D134" s="92" t="s">
         <v>17</v>
       </c>
@@ -7520,9 +7520,9 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="398"/>
+      <c r="A135" s="351"/>
       <c r="B135" s="212"/>
-      <c r="C135" s="395" t="s">
+      <c r="C135" s="348" t="s">
         <v>129</v>
       </c>
       <c r="D135" s="94" t="s">
@@ -7548,9 +7548,9 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="398"/>
+      <c r="A136" s="351"/>
       <c r="B136" s="212"/>
-      <c r="C136" s="396"/>
+      <c r="C136" s="349"/>
       <c r="D136" s="96" t="s">
         <v>17</v>
       </c>
@@ -7574,7 +7574,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="399"/>
+      <c r="A137" s="352"/>
       <c r="B137" s="213"/>
       <c r="C137" s="147" t="s">
         <v>131</v>
@@ -7602,7 +7602,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="379" t="s">
+      <c r="A138" s="402" t="s">
         <v>186</v>
       </c>
       <c r="B138" s="214"/>
@@ -7630,7 +7630,7 @@
       <c r="J138" s="306"/>
     </row>
     <row r="139" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A139" s="380"/>
+      <c r="A139" s="403"/>
       <c r="B139" s="215"/>
       <c r="C139" s="2" t="s">
         <v>188</v>
@@ -7656,7 +7656,7 @@
       <c r="J139" s="307"/>
     </row>
     <row r="140" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="381"/>
+      <c r="A140" s="404"/>
       <c r="B140" s="216"/>
       <c r="C140" s="20" t="s">
         <v>244</v>
@@ -7682,7 +7682,7 @@
       <c r="J140" s="308"/>
     </row>
     <row r="141" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A141" s="379" t="s">
+      <c r="A141" s="402" t="s">
         <v>192</v>
       </c>
       <c r="B141" s="214"/>
@@ -7710,7 +7710,7 @@
       <c r="J141" s="306"/>
     </row>
     <row r="142" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="380"/>
+      <c r="A142" s="403"/>
       <c r="B142" s="215"/>
       <c r="C142" s="329" t="s">
         <v>395</v>
@@ -7736,7 +7736,7 @@
       <c r="J142" s="307"/>
     </row>
     <row r="143" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="381"/>
+      <c r="A143" s="404"/>
       <c r="B143" s="217"/>
       <c r="C143" s="329" t="s">
         <v>396</v>
@@ -7846,7 +7846,7 @@
       <c r="J146" s="311"/>
     </row>
     <row r="147" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="374" t="s">
+      <c r="A147" s="400" t="s">
         <v>223</v>
       </c>
       <c r="B147" s="220" t="s">
@@ -7876,7 +7876,7 @@
       <c r="J147" s="312"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="375"/>
+      <c r="A148" s="401"/>
       <c r="B148" s="221" t="s">
         <v>248</v>
       </c>
@@ -9145,6 +9145,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="B28:B46"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B12:B27"/>
+    <mergeCell ref="A28:A51"/>
+    <mergeCell ref="C28:C41"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C91:C92"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="C102:C103"/>
@@ -9161,36 +9191,6 @@
     <mergeCell ref="C130:C134"/>
     <mergeCell ref="A97:A98"/>
     <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="B28:B46"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B12:B27"/>
-    <mergeCell ref="A28:A51"/>
-    <mergeCell ref="C28:C41"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C12:C23"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9202,7 +9202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADEA23E-E81E-4AF5-920B-9A516112A0D6}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -9222,22 +9222,22 @@
         <v>322</v>
       </c>
       <c r="B1" s="169" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C1" s="169" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D1" s="169" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="169" t="s">
+        <v>499</v>
+      </c>
+      <c r="F1" s="169" t="s">
         <v>500</v>
       </c>
-      <c r="F1" s="169" t="s">
-        <v>501</v>
-      </c>
       <c r="G1" s="169" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -9245,7 +9245,7 @@
         <v>374</v>
       </c>
       <c r="B2" s="169" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C2" s="169" t="s">
         <v>6</v>
@@ -9268,7 +9268,7 @@
         <v>376</v>
       </c>
       <c r="B3" s="169" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C3" s="169" t="s">
         <v>19</v>
@@ -9291,7 +9291,7 @@
         <v>385</v>
       </c>
       <c r="B4" s="169" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C4" s="169" t="s">
         <v>184</v>
@@ -9314,7 +9314,7 @@
         <v>385</v>
       </c>
       <c r="B5" s="169" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C5" s="169" t="s">
         <v>184</v>
@@ -9337,7 +9337,7 @@
         <v>378</v>
       </c>
       <c r="B6" s="169" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C6" s="169" t="s">
         <v>8</v>
@@ -9352,7 +9352,7 @@
         <v>42</v>
       </c>
       <c r="G6" s="169" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -9360,7 +9360,7 @@
         <v>378</v>
       </c>
       <c r="B7" s="169" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C7" s="169" t="s">
         <v>8</v>
@@ -9375,7 +9375,7 @@
         <v>42</v>
       </c>
       <c r="G7" s="169" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -9383,7 +9383,7 @@
         <v>378</v>
       </c>
       <c r="B8" s="169" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C8" s="169" t="s">
         <v>8</v>
@@ -9398,7 +9398,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="169" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -9406,7 +9406,7 @@
         <v>382</v>
       </c>
       <c r="B9" s="169" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C9" s="169" t="s">
         <v>14</v>
@@ -9429,13 +9429,13 @@
         <v>382</v>
       </c>
       <c r="B10" s="169" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C10" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="169" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E10" s="169">
         <v>628033</v>
@@ -9452,7 +9452,7 @@
         <v>381</v>
       </c>
       <c r="B11" s="169" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C11" s="169" t="s">
         <v>13</v>
@@ -9475,7 +9475,7 @@
         <v>381</v>
       </c>
       <c r="B12" s="169" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C12" s="169" t="s">
         <v>13</v>
@@ -9498,7 +9498,7 @@
         <v>379</v>
       </c>
       <c r="B13" s="169" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C13" s="169" t="s">
         <v>12</v>
@@ -9513,7 +9513,7 @@
         <v>58</v>
       </c>
       <c r="G13" s="169" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -9521,7 +9521,7 @@
         <v>379</v>
       </c>
       <c r="B14" s="169" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C14" s="169" t="s">
         <v>12</v>
@@ -9536,7 +9536,7 @@
         <v>58</v>
       </c>
       <c r="G14" s="169" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -9544,7 +9544,7 @@
         <v>386</v>
       </c>
       <c r="B15" s="169" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C15" s="169" t="s">
         <v>213</v>
@@ -9567,7 +9567,7 @@
         <v>386</v>
       </c>
       <c r="B16" s="169" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C16" s="169" t="s">
         <v>213</v>
@@ -9590,7 +9590,7 @@
         <v>384</v>
       </c>
       <c r="B17" s="169" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C17" s="169" t="s">
         <v>15</v>
@@ -9613,13 +9613,13 @@
         <v>384</v>
       </c>
       <c r="B18" s="169" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C18" s="169" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="169" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E18" s="169">
         <v>439396</v>
@@ -9636,7 +9636,7 @@
         <v>389</v>
       </c>
       <c r="B19" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C19" s="169" t="s">
         <v>336</v>
@@ -9651,7 +9651,7 @@
         <v>52</v>
       </c>
       <c r="G19" s="169" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
@@ -9659,7 +9659,7 @@
         <v>389</v>
       </c>
       <c r="B20" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C20" s="169" t="s">
         <v>339</v>
@@ -9674,7 +9674,7 @@
         <v>52</v>
       </c>
       <c r="G20" s="169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
@@ -9682,7 +9682,7 @@
         <v>389</v>
       </c>
       <c r="B21" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C21" s="169" t="s">
         <v>340</v>
@@ -9697,7 +9697,7 @@
         <v>52</v>
       </c>
       <c r="G21" s="169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
@@ -9705,7 +9705,7 @@
         <v>389</v>
       </c>
       <c r="B22" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C22" s="169" t="s">
         <v>358</v>
@@ -9720,7 +9720,7 @@
         <v>52</v>
       </c>
       <c r="G22" s="169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
@@ -9728,7 +9728,7 @@
         <v>389</v>
       </c>
       <c r="B23" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C23" s="169" t="s">
         <v>341</v>
@@ -9743,7 +9743,7 @@
         <v>52</v>
       </c>
       <c r="G23" s="169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
@@ -9751,7 +9751,7 @@
         <v>389</v>
       </c>
       <c r="B24" s="169" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C24" s="169" t="s">
         <v>343</v>
@@ -9766,15 +9766,15 @@
         <v>52</v>
       </c>
       <c r="G24" s="169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="169" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B25" s="169" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C25" s="169" t="s">
         <v>336</v>
@@ -9789,7 +9789,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="169" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -9797,7 +9797,7 @@
         <v>383</v>
       </c>
       <c r="B26" s="169" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C26" s="169" t="s">
         <v>20</v>
@@ -9842,10 +9842,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" t="s">
         <v>498</v>
-      </c>
-      <c r="B1" t="s">
-        <v>499</v>
       </c>
       <c r="C1" t="s">
         <v>371</v>
@@ -9867,7 +9867,7 @@
         <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C3" t="s">
         <v>390</v>
@@ -9875,10 +9875,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" t="s">
         <v>431</v>
-      </c>
-      <c r="B4" t="s">
-        <v>432</v>
       </c>
       <c r="C4" t="s">
         <v>231</v>
@@ -9897,10 +9897,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B6" t="s">
         <v>433</v>
-      </c>
-      <c r="B6" t="s">
-        <v>434</v>
       </c>
       <c r="C6" t="s">
         <v>241</v>
@@ -9908,10 +9908,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B7" t="s">
         <v>435</v>
-      </c>
-      <c r="B7" t="s">
-        <v>436</v>
       </c>
       <c r="C7" t="s">
         <v>92</v>
@@ -9919,10 +9919,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B8" t="s">
         <v>437</v>
-      </c>
-      <c r="B8" t="s">
-        <v>438</v>
       </c>
       <c r="C8" t="s">
         <v>238</v>
@@ -9930,10 +9930,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B9" t="s">
         <v>439</v>
-      </c>
-      <c r="B9" t="s">
-        <v>440</v>
       </c>
       <c r="C9" t="s">
         <v>85</v>
@@ -9941,10 +9941,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -9952,7 +9952,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B11" t="s">
         <v>170</v>
@@ -9966,7 +9966,7 @@
         <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C12" t="s">
         <v>215</v>
@@ -9977,7 +9977,7 @@
         <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C13" t="s">
         <v>244</v>
@@ -9985,10 +9985,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>443</v>
+      </c>
+      <c r="B14" t="s">
         <v>444</v>
-      </c>
-      <c r="B14" t="s">
-        <v>445</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -9996,10 +9996,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C15" t="s">
         <v>321</v>
@@ -10007,7 +10007,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
@@ -10018,10 +10018,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -10032,7 +10032,7 @@
         <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C18" t="s">
         <v>58</v>
@@ -10068,7 +10068,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -10079,7 +10079,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -10090,15 +10090,15 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B24" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -10109,7 +10109,7 @@
         <v>192</v>
       </c>
       <c r="B25" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C25" t="s">
         <v>396</v>
@@ -10120,10 +10120,10 @@
         <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -10131,7 +10131,7 @@
         <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C27" t="s">
         <v>61</v>
@@ -10139,10 +10139,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C28" t="s">
         <v>98</v>
@@ -10153,7 +10153,7 @@
         <v>192</v>
       </c>
       <c r="B29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C29" t="s">
         <v>191</v>
@@ -10164,7 +10164,7 @@
         <v>192</v>
       </c>
       <c r="B30" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C30" t="s">
         <v>395</v>
@@ -10172,10 +10172,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
@@ -10183,10 +10183,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C32" t="s">
         <v>132</v>
@@ -10194,10 +10194,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>457</v>
+      </c>
+      <c r="B33" t="s">
         <v>458</v>
-      </c>
-      <c r="B33" t="s">
-        <v>459</v>
       </c>
       <c r="C33" t="s">
         <v>103</v>
@@ -10208,7 +10208,7 @@
         <v>195</v>
       </c>
       <c r="B34" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C34" t="s">
         <v>196</v>
@@ -10216,10 +10216,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B35" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C35" t="s">
         <v>53</v>
@@ -10227,10 +10227,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>461</v>
+      </c>
+      <c r="B36" t="s">
         <v>462</v>
-      </c>
-      <c r="B36" t="s">
-        <v>463</v>
       </c>
       <c r="C36" t="s">
         <v>239</v>
@@ -10238,10 +10238,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>463</v>
+      </c>
+      <c r="B37" t="s">
         <v>464</v>
-      </c>
-      <c r="B37" t="s">
-        <v>465</v>
       </c>
       <c r="C37" t="s">
         <v>397</v>
@@ -10249,10 +10249,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C38" t="s">
         <v>197</v>
@@ -10260,10 +10260,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B39" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C39" t="s">
         <v>73</v>
@@ -10271,10 +10271,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>466</v>
+      </c>
+      <c r="B40" t="s">
         <v>467</v>
-      </c>
-      <c r="B40" t="s">
-        <v>468</v>
       </c>
       <c r="C40" t="s">
         <v>242</v>
@@ -10282,7 +10282,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B41" t="s">
         <v>173</v>
@@ -10293,7 +10293,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B42" t="s">
         <v>106</v>
@@ -10304,10 +10304,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>443</v>
+      </c>
+      <c r="B43" t="s">
         <v>444</v>
-      </c>
-      <c r="B43" t="s">
-        <v>445</v>
       </c>
       <c r="C43" t="s">
         <v>36</v>
@@ -10315,10 +10315,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B44" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C44" t="s">
         <v>199</v>
@@ -10326,13 +10326,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>470</v>
+      </c>
+      <c r="B45" t="s">
         <v>471</v>
       </c>
-      <c r="B45" t="s">
-        <v>472</v>
-      </c>
       <c r="C45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -10340,7 +10340,7 @@
         <v>139</v>
       </c>
       <c r="B46" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C46" t="s">
         <v>210</v>
@@ -10348,10 +10348,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>438</v>
+      </c>
+      <c r="B47" t="s">
         <v>439</v>
-      </c>
-      <c r="B47" t="s">
-        <v>440</v>
       </c>
       <c r="C47" t="s">
         <v>86</v>
@@ -10362,7 +10362,7 @@
         <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C48" t="s">
         <v>94</v>
@@ -10373,7 +10373,7 @@
         <v>192</v>
       </c>
       <c r="B49" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C49" t="s">
         <v>194</v>
@@ -10381,7 +10381,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B50" t="s">
         <v>175</v>
@@ -10395,7 +10395,7 @@
         <v>151</v>
       </c>
       <c r="B51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C51" t="s">
         <v>80</v>
@@ -10417,7 +10417,7 @@
         <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C53" t="s">
         <v>205</v>
@@ -10447,10 +10447,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C56" t="s">
         <v>23</v>
@@ -10461,7 +10461,7 @@
         <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C57" t="s">
         <v>123</v>
@@ -10472,7 +10472,7 @@
         <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C58" t="s">
         <v>214</v>
@@ -10483,7 +10483,7 @@
         <v>139</v>
       </c>
       <c r="B59" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C59" t="s">
         <v>217</v>
@@ -10505,7 +10505,7 @@
         <v>139</v>
       </c>
       <c r="B61" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C61" t="s">
         <v>54</v>
@@ -10524,7 +10524,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B63" t="s">
         <v>172</v>
@@ -10538,7 +10538,7 @@
         <v>139</v>
       </c>
       <c r="B64" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C64" t="s">
         <v>211</v>
@@ -10546,10 +10546,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B65" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C65" t="s">
         <v>245</v>
@@ -10557,10 +10557,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>443</v>
+      </c>
+      <c r="B66" t="s">
         <v>444</v>
-      </c>
-      <c r="B66" t="s">
-        <v>445</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
@@ -10568,10 +10568,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B67" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C67" t="s">
         <v>74</v>
@@ -10579,10 +10579,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C68" t="s">
         <v>198</v>
@@ -10601,7 +10601,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B70" t="s">
         <v>224</v>
@@ -10612,7 +10612,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B71" t="s">
         <v>154</v>
@@ -10623,7 +10623,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B72" t="s">
         <v>124</v>
@@ -10637,7 +10637,7 @@
         <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C73" t="s">
         <v>68</v>
@@ -10648,7 +10648,7 @@
         <v>140</v>
       </c>
       <c r="B74" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C74" t="s">
         <v>64</v>
@@ -10656,10 +10656,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B75" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C75" t="s">
         <v>71</v>
@@ -10667,10 +10667,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B76" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C76" t="s">
         <v>357</v>
@@ -10678,10 +10678,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B77" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C77" t="s">
         <v>89</v>
@@ -10692,7 +10692,7 @@
         <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C78" t="s">
         <v>83</v>
@@ -10700,7 +10700,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B79" t="s">
         <v>169</v>
@@ -10711,10 +10711,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B80" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C80" t="s">
         <v>391</v>
@@ -10722,10 +10722,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B81" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C81" t="s">
         <v>49</v>
@@ -10744,10 +10744,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>488</v>
+      </c>
+      <c r="B83" t="s">
         <v>489</v>
-      </c>
-      <c r="B83" t="s">
-        <v>490</v>
       </c>
       <c r="C83" t="s">
         <v>240</v>
@@ -10755,10 +10755,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>490</v>
+      </c>
+      <c r="B84" t="s">
         <v>491</v>
-      </c>
-      <c r="B84" t="s">
-        <v>492</v>
       </c>
       <c r="C84" t="s">
         <v>188</v>
@@ -10777,10 +10777,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B86" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C86" t="s">
         <v>41</v>
@@ -10791,7 +10791,7 @@
         <v>140</v>
       </c>
       <c r="B87" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C87" t="s">
         <v>69</v>
@@ -10802,7 +10802,7 @@
         <v>159</v>
       </c>
       <c r="B88" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C88" t="s">
         <v>96</v>
@@ -10810,10 +10810,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B89" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C89" t="s">
         <v>187</v>
@@ -10821,10 +10821,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C90" t="s">
         <v>45</v>
@@ -10832,10 +10832,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>443</v>
+      </c>
+      <c r="B91" t="s">
         <v>444</v>
-      </c>
-      <c r="B91" t="s">
-        <v>445</v>
       </c>
       <c r="C91" t="s">
         <v>201</v>
@@ -10846,7 +10846,7 @@
         <v>140</v>
       </c>
       <c r="B92" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C92" t="s">
         <v>63</v>
@@ -10854,10 +10854,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C93" t="s">
         <v>32</v>
@@ -10865,10 +10865,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>495</v>
+      </c>
+      <c r="B94" t="s">
         <v>496</v>
-      </c>
-      <c r="B94" t="s">
-        <v>497</v>
       </c>
       <c r="C94" t="s">
         <v>125</v>
@@ -10876,10 +10876,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>495</v>
+      </c>
+      <c r="B95" t="s">
         <v>496</v>
-      </c>
-      <c r="B95" t="s">
-        <v>497</v>
       </c>
       <c r="C95" t="s">
         <v>131</v>
@@ -10887,10 +10887,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>495</v>
+      </c>
+      <c r="B96" t="s">
         <v>496</v>
-      </c>
-      <c r="B96" t="s">
-        <v>497</v>
       </c>
       <c r="C96" t="s">
         <v>129</v>
@@ -10898,7 +10898,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B97" t="s">
         <v>222</v>
@@ -10909,7 +10909,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B98" t="s">
         <v>208</v>
@@ -11094,7 +11094,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="332" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B20" s="167" t="s">
         <v>364</v>
@@ -11105,7 +11105,7 @@
         <v>372</v>
       </c>
       <c r="B21" s="330" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -11126,7 +11126,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B24" s="167" t="s">
         <v>252</v>
@@ -11286,7 +11286,7 @@
     </row>
     <row r="44" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B44" t="s">
         <v>320</v>
@@ -11406,7 +11406,7 @@
     </row>
     <row r="59" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B59" s="168" t="s">
         <v>367</v>
@@ -11414,7 +11414,7 @@
     </row>
     <row r="60" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B60" s="168" t="s">
         <v>368</v>

</xml_diff>